<commit_message>
update excel files for test_data
</commit_message>
<xml_diff>
--- a/template_files/template_no_gui.xlsx
+++ b/template_files/template_no_gui.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/NET_v2.24/template_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/net/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881FE4D9-13C8-E143-A1EA-541C19874C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A715293-7A80-674E-AE1D-285EEE60271D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="13000" windowHeight="14580" tabRatio="401" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="760" windowWidth="13000" windowHeight="14580" tabRatio="401" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -7734,8 +7734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7922,7 +7922,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="C18" s="69" t="s">
         <v>89</v>
@@ -9081,7 +9081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove fsn as head modelling method
</commit_message>
<xml_diff>
--- a/template_files/template_no_gui.xlsx
+++ b/template_files/template_no_gui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/net/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A715293-7A80-674E-AE1D-285EEE60271D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BC32C2-F1D1-5B49-AD88-19882C7677BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="13000" windowHeight="14580" tabRatio="401" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12360" yWindow="1500" windowWidth="13000" windowHeight="14580" tabRatio="401" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -202,9 +202,6 @@
     <t>leadfield.method</t>
   </si>
   <si>
-    <t>string - Method for head model -  dipoli, simbio, fns, gfdm</t>
-  </si>
-  <si>
     <t>leadfield.input_voxel_size</t>
   </si>
   <si>
@@ -896,6 +893,9 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>string - Method for head model -  gfdm, simbio, dipoli</t>
   </si>
 </sst>
 </file>
@@ -7284,14 +7284,14 @@
     </row>
     <row r="2" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>255</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>10</v>
@@ -7306,7 +7306,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>10</v>
@@ -7400,7 +7400,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>15</v>
@@ -7444,7 +7444,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="145" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>23</v>
@@ -7470,11 +7470,11 @@
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -7569,8 +7569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -7608,7 +7608,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>38</v>
@@ -7619,7 +7619,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>40</v>
@@ -7641,7 +7641,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>45</v>
@@ -7663,7 +7663,7 @@
         <v>49</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>50</v>
@@ -7674,7 +7674,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>52</v>
@@ -7696,32 +7696,32 @@
         <v>55</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>56</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="40">
         <v>2</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="42">
         <v>6</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -7734,7 +7734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -7759,95 +7759,95 @@
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="50" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="49">
         <v>3</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="33">
         <v>1</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="33">
         <v>80</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="C8" s="57" t="s">
         <v>75</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="C9" s="60" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="59">
         <v>5</v>
@@ -7856,7 +7856,7 @@
     </row>
     <row r="11" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="59">
         <v>36</v>
@@ -7865,7 +7865,7 @@
     </row>
     <row r="12" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="59">
         <v>80</v>
@@ -7874,7 +7874,7 @@
     </row>
     <row r="13" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="59">
         <v>10</v>
@@ -7883,7 +7883,7 @@
     </row>
     <row r="14" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="59">
         <v>30</v>
@@ -7892,7 +7892,7 @@
     </row>
     <row r="15" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="59">
         <v>0</v>
@@ -7901,16 +7901,16 @@
     </row>
     <row r="16" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="65">
         <v>258</v>
@@ -7919,431 +7919,431 @@
     </row>
     <row r="18" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="68" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="49">
         <v>200</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="C21" s="75" t="s">
         <v>95</v>
-      </c>
-      <c r="C21" s="75" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="74">
         <v>1</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="74">
         <v>5</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="73" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="74">
         <v>12</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="74">
         <v>0.2</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="77" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="80" t="s">
+      <c r="C29" s="81" t="s">
         <v>112</v>
-      </c>
-      <c r="C29" s="81" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="80">
         <v>1</v>
       </c>
       <c r="C30" s="81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B31" s="80">
         <v>7</v>
       </c>
       <c r="C31" s="81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" s="82" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="80">
         <v>30</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B34" s="80">
         <v>0.8</v>
       </c>
       <c r="C34" s="81" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="76" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="82" t="s">
         <v>10</v>
       </c>
       <c r="C35" s="78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="80">
         <v>0.2</v>
       </c>
       <c r="C36" s="81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37" s="83" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="74" t="s">
+      <c r="C38" s="75" t="s">
         <v>130</v>
-      </c>
-      <c r="C38" s="75" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="74">
         <v>1</v>
       </c>
       <c r="C39" s="75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="70" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="83" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="74">
         <v>0.5</v>
       </c>
       <c r="C41" s="75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" s="83" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="14" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B43" s="74">
         <v>0.2</v>
       </c>
       <c r="C43" s="75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="129" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B44" s="130" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="131" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="132" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B45" s="133" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="134" t="s">
         <v>95</v>
-      </c>
-      <c r="C45" s="134" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="132" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B46" s="133">
         <v>1</v>
       </c>
       <c r="C46" s="134" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="129" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B47" s="135" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="131" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="132" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B48" s="133">
         <v>1</v>
       </c>
       <c r="C48" s="134" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="129" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B49" s="135" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="131" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="132" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B50" s="133">
         <v>0.2</v>
       </c>
       <c r="C50" s="134" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B51" s="68" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B52" s="49">
         <v>0.2</v>
       </c>
       <c r="C52" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="30" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="C54" s="54" t="s">
         <v>146</v>
-      </c>
-      <c r="B54" s="33" t="s">
-        <v>282</v>
-      </c>
-      <c r="C54" s="54" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="69" t="s">
         <v>148</v>
-      </c>
-      <c r="B55" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="69" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="84" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B56" s="85">
         <v>200</v>
       </c>
       <c r="C56" s="86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -8388,51 +8388,51 @@
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>152</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A3" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="69" t="s">
         <v>154</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A4" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="87">
         <v>0.5</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A5" s="67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="69" t="s">
         <v>152</v>
-      </c>
-      <c r="C5" s="69" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A6" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="68">
         <v>4</v>
@@ -8441,7 +8441,7 @@
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A7" s="67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="68">
         <v>8</v>
@@ -8450,29 +8450,29 @@
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A8" s="67" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>282</v>
+      </c>
+      <c r="C8" s="69" t="s">
         <v>161</v>
-      </c>
-      <c r="B8" s="68" t="s">
-        <v>283</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A9" s="88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" s="89">
         <v>0.05</v>
       </c>
       <c r="C9" s="90" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A10" s="91" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="92">
         <v>0</v>
@@ -8481,7 +8481,7 @@
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A11" s="91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" s="92">
         <v>100</v>
@@ -8490,18 +8490,18 @@
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A12" s="94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="96" t="s">
         <v>152</v>
-      </c>
-      <c r="C12" s="96" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A13" s="94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" s="95">
         <v>5</v>
@@ -8510,18 +8510,18 @@
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A14" s="94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="96" t="s">
         <v>152</v>
-      </c>
-      <c r="C14" s="96" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A15" s="94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="95">
         <v>0.1</v>
@@ -8530,7 +8530,7 @@
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A16" s="94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="95">
         <v>0</v>
@@ -8539,7 +8539,7 @@
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A17" s="97" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="98">
         <v>10</v>
@@ -8548,7 +8548,7 @@
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A18" s="97" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="98">
         <v>5</v>
@@ -8557,7 +8557,7 @@
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A19" s="97" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" s="98">
         <v>1</v>
@@ -8566,7 +8566,7 @@
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A20" s="100" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20" s="101">
         <v>0.05</v>
@@ -8575,13 +8575,13 @@
     </row>
     <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A21" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="104" t="s">
         <v>176</v>
       </c>
-      <c r="B21" s="104" t="s">
+      <c r="C21" s="105" t="s">
         <v>177</v>
-      </c>
-      <c r="C21" s="105" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.15">
@@ -8663,156 +8663,156 @@
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>179</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.15">
       <c r="A4" s="107" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="108" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="109" t="s">
         <v>182</v>
-      </c>
-      <c r="B4" s="108" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="109" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="49">
         <v>1</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="49">
         <v>80</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.15">
       <c r="A8" s="110" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="112" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" s="111" t="s">
-        <v>285</v>
-      </c>
-      <c r="C8" s="112" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10" s="82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.15">
       <c r="A11" s="113" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="114" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="76" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="80">
         <v>1</v>
       </c>
       <c r="C13" s="81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B14" s="80">
         <v>80</v>
       </c>
       <c r="C14" s="81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.15">
       <c r="A15" s="116" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="118" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -8857,211 +8857,211 @@
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" s="49">
         <v>1</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="49">
         <v>80</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="49">
         <v>2</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="49">
         <v>1</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" s="49">
         <v>6</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="C8" s="50" t="s">
         <v>209</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="119" t="s">
         <v>211</v>
       </c>
-      <c r="B9" s="119" t="s">
+      <c r="C9" s="50" t="s">
         <v>212</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="C10" s="50" t="s">
         <v>215</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.15">
       <c r="A11" s="136" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C11" s="138" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" s="82" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" s="82" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="79" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="120">
         <v>2</v>
       </c>
       <c r="C14" s="81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="79" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B15" s="120">
         <v>1</v>
       </c>
       <c r="C15" s="81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.15">
       <c r="A16" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="B16" s="114" t="s">
+      <c r="C16" s="121" t="s">
         <v>222</v>
-      </c>
-      <c r="C16" s="121" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="113" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="114" t="s">
         <v>224</v>
       </c>
-      <c r="B17" s="114" t="s">
+      <c r="C17" s="115" t="s">
         <v>225</v>
-      </c>
-      <c r="C17" s="115" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B18" s="122">
         <v>1000</v>
       </c>
       <c r="C18" s="115" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.15">
       <c r="A19" s="142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B19" s="143" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C19" s="144" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.15">
       <c r="A20" s="139" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="140" t="s">
+        <v>284</v>
+      </c>
+      <c r="C20" s="141" t="s">
         <v>274</v>
-      </c>
-      <c r="B20" s="140" t="s">
-        <v>285</v>
-      </c>
-      <c r="C20" s="141" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -9106,123 +9106,123 @@
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="123" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="123" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="123" t="s">
+      <c r="C2" s="124" t="s">
         <v>231</v>
-      </c>
-      <c r="C2" s="124" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="123" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="128" t="s">
         <v>233</v>
-      </c>
-      <c r="B3" s="123" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" s="128" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="125" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="125" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="125" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="125" t="s">
         <v>238</v>
-      </c>
-      <c r="B5" s="125" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="125" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="125" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="125" t="s">
         <v>240</v>
-      </c>
-      <c r="B6" s="125" t="s">
-        <v>236</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="125" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="125" t="s">
         <v>242</v>
-      </c>
-      <c r="B7" s="125" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="125" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="125" t="s">
         <v>244</v>
-      </c>
-      <c r="B8" s="125" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="123" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="123" t="s">
         <v>246</v>
       </c>
-      <c r="B9" s="123" t="s">
+      <c r="C9" s="126" t="s">
         <v>247</v>
-      </c>
-      <c r="C9" s="126" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="123" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B10" s="123">
         <v>5000</v>
       </c>
       <c r="C10" s="123" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="123" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11" s="123">
         <v>0.05</v>
       </c>
       <c r="C11" s="126" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="127" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="127" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="127" t="s">
         <v>253</v>
-      </c>
-      <c r="B12" s="127" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="127" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move the statistical part in a new sub-function
</commit_message>
<xml_diff>
--- a/template_files/template_no_gui.xlsx
+++ b/template_files/template_no_gui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/NET_v2.24/template_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/net/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881FE4D9-13C8-E143-A1EA-541C19874C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DAE8C6-E0E7-964D-892F-8380A5396F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="13000" windowHeight="14580" tabRatio="401" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="760" windowWidth="13000" windowHeight="14580" tabRatio="401" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="287">
   <si>
     <t>eeg_filename</t>
   </si>
@@ -886,16 +886,13 @@
     <t>eloreta</t>
   </si>
   <si>
-    <t>test_seeds</t>
-  </si>
-  <si>
-    <t>test_template_erp</t>
-  </si>
-  <si>
-    <t>test_template_ers_erd</t>
-  </si>
-  <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>template_seeds</t>
+  </si>
+  <si>
+    <t>template_10_July</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +1864,35 @@
     <cellStyle name="Standaard 6" xfId="4" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="Standaard 7" xfId="5" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -7350,16 +7375,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"on"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"on"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"on"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8348,10 +8373,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"on"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8622,10 +8647,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8639,7 +8664,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -8688,7 +8713,7 @@
         <v>182</v>
       </c>
       <c r="B4" s="108" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C4" s="109" t="s">
         <v>183</v>
@@ -8732,7 +8757,7 @@
         <v>189</v>
       </c>
       <c r="B8" s="111" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C8" s="112" t="s">
         <v>190</v>
@@ -8764,8 +8789,8 @@
       <c r="A11" s="113" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="114" t="s">
-        <v>284</v>
+      <c r="B11" s="143" t="s">
+        <v>285</v>
       </c>
       <c r="C11" s="115" t="s">
         <v>183</v>
@@ -8816,12 +8841,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="B1:B10 B12:B1048576">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"on"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="off">
+      <formula>LEFT(B11,LEN("off"))="off"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="on">
+      <formula>LEFT(B11,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8832,8 +8865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -9047,7 +9080,7 @@
         <v>229</v>
       </c>
       <c r="B19" s="143" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C19" s="144" t="s">
         <v>183</v>
@@ -9058,19 +9091,27 @@
         <v>274</v>
       </c>
       <c r="B20" s="140" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C20" s="141" t="s">
         <v>275</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="off">
+  <conditionalFormatting sqref="B1:B18 B20:B1048576">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="off">
       <formula>NOT(ISERROR(SEARCH("off",B1)))</formula>
     </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="4" operator="beginsWith" text="on">
+      <formula>LEFT(B1,LEN("on"))="on"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="off">
+      <formula>LEFT(B19,LEN("off"))="off"</formula>
+    </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="on">
-      <formula>LEFT(B1,LEN("on"))="on"</formula>
+      <formula>LEFT(B19,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9081,7 +9122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9120,7 +9161,7 @@
         <v>233</v>
       </c>
       <c r="B3" s="123" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C3" s="128" t="s">
         <v>234</v>
@@ -9227,10 +9268,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="no">
+    <cfRule type="beginsWith" dxfId="5" priority="1" operator="beginsWith" text="no">
       <formula>LEFT(B1,LEN("no"))="no"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="yes">
+    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="yes">
       <formula>LEFT(B1,LEN("yes"))="yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>